<commit_message>
Backup slides are added.
</commit_message>
<xml_diff>
--- a/ConfidenceInterval/12_4_4.xlsx
+++ b/ConfidenceInterval/12_4_4.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="12_4_4" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -845,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3729,20 +3729,34 @@
         <f>AVERAGE(C1:C99)</f>
         <v>0.16182131313131312</v>
       </c>
+      <c r="D101">
+        <f>AVERAGE(D1:D99)</f>
+        <v>2.304266161616161E-2</v>
+      </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C102">
         <f>STDEV(C1:C99)</f>
         <v>4.9743487106178857E-3</v>
       </c>
+      <c r="D102">
+        <f>STDEV(D1:D99)</f>
+        <v>8.4457721674353675E-4</v>
+      </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C103">
         <v>0.16084119999999999</v>
       </c>
+      <c r="D103">
+        <v>0.16084119999999999</v>
+      </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C104">
+        <v>0.1628008</v>
+      </c>
+      <c r="D104">
         <v>0.1628008</v>
       </c>
     </row>
@@ -3751,16 +3765,42 @@
         <f>C101-C103</f>
         <v>9.8011313131313171E-4</v>
       </c>
+      <c r="D105">
+        <v>2.2873689999999999E-2</v>
+      </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C106">
         <f>C104-C101</f>
         <v>9.7948686868687407E-4</v>
       </c>
+      <c r="D106">
+        <v>2.3210310000000001E-2</v>
+      </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C107">
         <v>1E-3</v>
+      </c>
+      <c r="D107">
+        <f>D105-D106</f>
+        <v>-3.3662000000000275E-4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>2.2819209999999999E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>2.326479E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <f>D110-D109</f>
+        <v>4.4558000000000098E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>